<commit_message>
updated design, new test app, ready for assembly
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\Electronics\WS2811 Expander\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A8D3DA-AD01-416A-9E3E-770EF055E304}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3992AF5D-42D1-4AE4-81A8-6805A002F939}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1176" windowWidth="18276" windowHeight="15192" activeTab="1" xr2:uid="{C90114B8-4AD5-44F7-8BE0-F428A7AE3971}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="28380" windowHeight="15396" xr2:uid="{C90114B8-4AD5-44F7-8BE0-F428A7AE3971}"/>
   </bookViews>
   <sheets>
     <sheet name="Board" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="110">
   <si>
     <t>WS2811 expander BOM</t>
   </si>
@@ -305,12 +306,6 @@
     <t>Desired to make</t>
   </si>
   <si>
-    <t>erj-6geyj102v</t>
-  </si>
-  <si>
-    <t>ERJ-6GEYJ103V</t>
-  </si>
-  <si>
     <t>ERJ-6GEYJ272V</t>
   </si>
   <si>
@@ -330,16 +325,56 @@
   </si>
   <si>
     <t>lcsc.com</t>
+  </si>
+  <si>
+    <t>CRCW080510K0JNEAC</t>
+  </si>
+  <si>
+    <t>CRCW08051K00JNEAC</t>
+  </si>
+  <si>
+    <t>lcsc</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>newark</t>
+  </si>
+  <si>
+    <t>newark order used different numbers</t>
+  </si>
+  <si>
+    <t>allpcb assembled</t>
+  </si>
+  <si>
+    <t>Joints</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Setup</t>
+  </si>
+  <si>
+    <t>Stencil</t>
+  </si>
+  <si>
+    <t>Assembly</t>
+  </si>
+  <si>
+    <t>board total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,6 +395,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -383,7 +424,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -392,6 +433,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -707,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC583114-D5AA-4471-918E-3F49F4519113}">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:R67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34:O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -720,22 +765,27 @@
     <col min="4" max="4" width="12.5546875" customWidth="1"/>
     <col min="5" max="5" width="25.77734375" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" customWidth="1"/>
+    <col min="16" max="16" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>48</v>
       </c>
       <c r="F3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="O3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -758,7 +808,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -782,8 +832,10 @@
       <c r="H5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -810,8 +862,15 @@
       <c r="H6" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="O6" s="3">
+        <v>5.96E-2</v>
+      </c>
+      <c r="P6" s="3">
+        <f t="shared" ref="P6:P14" si="0">O6*A6</f>
+        <v>5.96E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -828,18 +887,25 @@
         <v>0.15</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" ref="F7:F14" si="0">$A7*D7</f>
+        <f t="shared" ref="F7:F14" si="1">$A7*D7</f>
         <v>1.32</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" ref="G7:G14" si="1">$A7*E7</f>
+        <f t="shared" ref="G7:G14" si="2">$A7*E7</f>
         <v>0.44999999999999996</v>
       </c>
       <c r="H7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="O7" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="P7" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0499999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -856,186 +922,235 @@
         <v>0.01</v>
       </c>
       <c r="F8" s="3">
+        <f t="shared" si="1"/>
+        <v>0.09</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="2"/>
+        <v>0.03</v>
+      </c>
+      <c r="H8" t="s">
+        <v>84</v>
+      </c>
+      <c r="O8" s="3">
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="P8" s="3">
         <f t="shared" si="0"/>
-        <v>0.09</v>
-      </c>
-      <c r="G8" s="3">
+        <v>4.4400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="1"/>
+        <v>0.08</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="H9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O9" s="3">
+        <v>1.78E-2</v>
+      </c>
+      <c r="P9" s="3">
+        <f t="shared" si="0"/>
+        <v>1.78E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="H10" t="s">
+        <v>84</v>
+      </c>
+      <c r="O10" s="3">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="P10" s="3">
+        <f t="shared" si="0"/>
+        <v>2.7000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="H11" t="s">
+        <v>84</v>
+      </c>
+      <c r="O11" s="3">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="P11" s="3">
+        <f t="shared" si="0"/>
+        <v>2.7000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="H12" t="s">
+        <v>84</v>
+      </c>
+      <c r="O12" s="3">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="P12" s="3">
+        <f t="shared" si="0"/>
+        <v>2.7000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="1"/>
+        <v>0.06</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="2"/>
+        <v>0.06</v>
+      </c>
+      <c r="H13" t="s">
+        <v>84</v>
+      </c>
+      <c r="O13" s="3">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="P13" s="3">
+        <f t="shared" si="0"/>
+        <v>1.6199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="F14" s="3">
         <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
-      <c r="H8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0.08</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="F9" s="3">
-        <f t="shared" si="0"/>
-        <v>0.08</v>
-      </c>
-      <c r="G9" s="3">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
-      </c>
-      <c r="H9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="F10" s="3">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-      <c r="G10" s="3">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
-      </c>
-      <c r="H10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="F11" s="3">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-      <c r="G11" s="3">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
-      </c>
-      <c r="H11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="F12" s="3">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-      <c r="G12" s="3">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
-      </c>
-      <c r="H12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="F13" s="3">
-        <f t="shared" si="0"/>
-        <v>0.06</v>
-      </c>
-      <c r="G13" s="3">
-        <f t="shared" si="1"/>
-        <v>0.06</v>
-      </c>
-      <c r="H13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>3</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="F14" s="3">
-        <f t="shared" si="0"/>
-        <v>0.03</v>
-      </c>
       <c r="G14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.03</v>
       </c>
       <c r="H14" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="O14" s="3">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="P14" s="3">
+        <f t="shared" si="0"/>
+        <v>8.0999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3">
@@ -1049,8 +1164,27 @@
       <c r="H15" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="P15" s="3">
+        <f>SUM(P5:P14)</f>
+        <v>1.2041999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L17" t="s">
+        <v>104</v>
+      </c>
+      <c r="M17">
+        <v>52</v>
+      </c>
+      <c r="N17" s="3">
+        <v>1.5E-3</v>
+      </c>
+      <c r="P17" s="3">
+        <f>M17*N17</f>
+        <v>7.8E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1064,15 +1198,15 @@
         <v>0.1</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" ref="F18:F20" si="2">$A18*D18</f>
+        <f t="shared" ref="F18:F20" si="3">$A18*D18</f>
         <v>0.38</v>
       </c>
       <c r="G18" s="3">
-        <f t="shared" ref="G18:G20" si="3">$A18*E18</f>
+        <f t="shared" ref="G18:G20" si="4">$A18*E18</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1086,15 +1220,19 @@
         <v>0.03</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="G19" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.03</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="P19" s="3">
+        <f>P15+P17</f>
+        <v>1.2821999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1108,15 +1246,15 @@
         <v>0.03</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.03</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="F21" s="3">
         <f>SUM(F18:F20)</f>
         <v>0.67</v>
@@ -1126,7 +1264,31 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L22" t="s">
+        <v>105</v>
+      </c>
+      <c r="M22">
+        <v>1000</v>
+      </c>
+      <c r="P22" s="3">
+        <f>M22 * P19</f>
+        <v>1282.1999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L23" t="s">
+        <v>106</v>
+      </c>
+      <c r="M23" s="7">
+        <v>7</v>
+      </c>
+      <c r="P23" s="7">
+        <f>M23</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -1138,16 +1300,36 @@
         <f>G15+G21</f>
         <v>1.21</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="L24" t="s">
+        <v>72</v>
+      </c>
+      <c r="M24" s="7">
+        <v>3</v>
+      </c>
+      <c r="P24" s="7">
+        <f>M24</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>19</v>
       </c>
       <c r="D25" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="L25" t="s">
+        <v>107</v>
+      </c>
+      <c r="M25" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="P25" s="7">
+        <f>M25</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>20</v>
       </c>
@@ -1157,13 +1339,21 @@
       <c r="D26" s="3">
         <v>0.59</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="P26" s="3">
+        <f>SUM(P22:P25)</f>
+        <v>1293.6999999999998</v>
+      </c>
+      <c r="R26" s="3">
+        <f>P26/M22</f>
+        <v>1.2936999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>22</v>
       </c>
@@ -1174,7 +1364,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -1182,7 +1372,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>29</v>
       </c>
@@ -1192,8 +1382,23 @@
       <c r="D32" s="3">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I32" t="s">
+        <v>109</v>
+      </c>
+      <c r="L32" t="s">
+        <v>86</v>
+      </c>
+      <c r="M32" t="s">
+        <v>108</v>
+      </c>
+      <c r="N32" t="s">
+        <v>31</v>
+      </c>
+      <c r="O32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>30</v>
       </c>
@@ -1203,8 +1408,29 @@
       <c r="D33" s="3">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I33" s="7">
+        <v>5</v>
+      </c>
+      <c r="K33">
+        <v>10</v>
+      </c>
+      <c r="L33" s="3">
+        <f>I33/K33</f>
+        <v>0.5</v>
+      </c>
+      <c r="M33" s="3">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="N33" s="3">
+        <f>L33+M33</f>
+        <v>2.93</v>
+      </c>
+      <c r="O33" s="3">
+        <f>N33*K33</f>
+        <v>29.3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>27</v>
       </c>
@@ -1214,8 +1440,29 @@
       <c r="D34" s="3">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I34" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="K34">
+        <v>25</v>
+      </c>
+      <c r="L34" s="3">
+        <f t="shared" ref="L34:L37" si="5">I34/K34</f>
+        <v>0.22399999999999998</v>
+      </c>
+      <c r="M34" s="3">
+        <v>1.74</v>
+      </c>
+      <c r="N34" s="3">
+        <f t="shared" ref="N34:N37" si="6">L34+M34</f>
+        <v>1.964</v>
+      </c>
+      <c r="O34" s="3">
+        <f t="shared" ref="O34:O37" si="7">N34*K34</f>
+        <v>49.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>32</v>
       </c>
@@ -1228,13 +1475,78 @@
       <c r="F35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I35" s="3">
+        <v>12.1</v>
+      </c>
+      <c r="K35">
+        <v>100</v>
+      </c>
+      <c r="L35" s="3">
+        <f t="shared" si="5"/>
+        <v>0.121</v>
+      </c>
+      <c r="M35" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="N35" s="3">
+        <f t="shared" si="6"/>
+        <v>1.5209999999999999</v>
+      </c>
+      <c r="O35" s="3">
+        <f t="shared" si="7"/>
+        <v>152.1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="I36" s="3">
+        <v>28.2</v>
+      </c>
+      <c r="K36">
+        <v>500</v>
+      </c>
+      <c r="L36" s="3">
+        <f t="shared" si="5"/>
+        <v>5.6399999999999999E-2</v>
+      </c>
+      <c r="M36" s="3">
+        <v>1.31</v>
+      </c>
+      <c r="N36" s="3">
+        <f t="shared" si="6"/>
+        <v>1.3664000000000001</v>
+      </c>
+      <c r="O36" s="3">
+        <f t="shared" si="7"/>
+        <v>683.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I37" s="3">
+        <v>48.4</v>
+      </c>
+      <c r="K37">
+        <v>1000</v>
+      </c>
+      <c r="L37" s="3">
+        <f t="shared" si="5"/>
+        <v>4.8399999999999999E-2</v>
+      </c>
+      <c r="M37" s="3">
+        <v>1.29</v>
+      </c>
+      <c r="N37" s="3">
+        <f t="shared" si="6"/>
+        <v>1.3384</v>
+      </c>
+      <c r="O37" s="3">
+        <f t="shared" si="7"/>
+        <v>1338.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>37</v>
       </c>
@@ -1242,7 +1554,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>32</v>
       </c>
@@ -1250,7 +1562,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>38</v>
       </c>
@@ -1261,16 +1573,16 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C41" s="2"/>
       <c r="D41" s="3"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>38</v>
       </c>
@@ -1281,7 +1593,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>37</v>
       </c>
@@ -1290,7 +1602,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>27</v>
       </c>
@@ -1299,7 +1611,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -1435,35 +1747,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B6CC41B-053E-4F9B-818B-1489A13B117E}">
-  <dimension ref="A2:L15"/>
+  <dimension ref="A2:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="25.109375" customWidth="1"/>
     <col min="3" max="3" width="12.77734375" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="11.21875" customWidth="1"/>
-    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="I3" t="s">
         <v>89</v>
       </c>
       <c r="K3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L4" t="s">
+        <v>101</v>
+      </c>
+      <c r="M4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -1474,10 +1795,10 @@
         <v>86</v>
       </c>
       <c r="L5" s="5">
-        <v>43601</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+        <v>43758</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1485,21 +1806,18 @@
         <v>17</v>
       </c>
       <c r="E6">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="G6">
         <f>E6/A6</f>
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="J6">
         <f>K$3*A6 - E6</f>
         <v>0</v>
       </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1507,24 +1825,24 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="G7">
         <f t="shared" ref="G7:G15" si="0">E7/A7</f>
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="J7">
         <f t="shared" ref="J7:J15" si="1">K$3*A7 - E7</f>
-        <v>19</v>
-      </c>
-      <c r="L7">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1535,24 +1853,21 @@
         <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E8">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>6.666666666666667</v>
+        <v>19.666666666666668</v>
       </c>
       <c r="J8">
         <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="L8">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1563,24 +1878,27 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E9">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>7.333333333333333</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="J9">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>139</v>
       </c>
       <c r="L9">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+      <c r="N9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1588,21 +1906,27 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E10">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="J10">
         <f t="shared" si="1"/>
-        <v>-76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+        <v>-20</v>
+      </c>
+      <c r="L10">
+        <v>100</v>
+      </c>
+      <c r="N10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1613,21 +1937,27 @@
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E11">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="J11">
         <f t="shared" si="1"/>
-        <v>-14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="L11">
+        <v>100</v>
+      </c>
+      <c r="N11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1638,21 +1968,27 @@
         <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E12">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="J12">
         <f t="shared" si="1"/>
-        <v>-14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="L12">
+        <v>100</v>
+      </c>
+      <c r="N12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1663,21 +1999,27 @@
         <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E13">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="J13">
         <f t="shared" si="1"/>
-        <v>-14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="L13">
+        <v>100</v>
+      </c>
+      <c r="N13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1687,25 +2029,29 @@
       <c r="C14" t="s">
         <v>32</v>
       </c>
-      <c r="D14" t="s">
-        <v>91</v>
+      <c r="D14" s="6" t="s">
+        <v>97</v>
       </c>
       <c r="E14">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="J14">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>135</v>
       </c>
       <c r="L14">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+      <c r="M14" s="6"/>
+      <c r="N14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>6</v>
       </c>
@@ -1716,25 +2062,31 @@
         <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E15">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>0.83333333333333337</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="J15">
         <f t="shared" si="1"/>
-        <v>115</v>
+        <v>266</v>
       </c>
       <c r="L15">
-        <v>150</v>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>